<commit_message>
Update the RaceOfPersonType code table.
</commit_message>
<xml_diff>
--- a/tools/nibrs-staging-data/src/test/resources/codeSpreadSheets/NIBRSCodeTablesHawaii.xlsx
+++ b/tools/nibrs-staging-data/src/test/resources/codeSpreadSheets/NIBRSCodeTablesHawaii.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haiqiwei/git/nibrsSpringBoot2/tools/nibrs-staging-data/src/test/resources/codeSpreadSheets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD351DF-BDCF-C74F-A07B-FB335FF7E370}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21680" yWindow="1660" windowWidth="24880" windowHeight="14800" tabRatio="705" firstSheet="22" activeTab="24"/>
+    <workbookView xWindow="44480" yWindow="1920" windowWidth="24880" windowHeight="14800" tabRatio="705" firstSheet="15" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -40,7 +46,7 @@
     <sheet name="CargoTheftIndicatorType" sheetId="31" r:id="rId31"/>
     <sheet name="Agency" sheetId="32" r:id="rId32"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -50,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2347" uniqueCount="733">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="731">
   <si>
     <t>Table</t>
   </si>
@@ -2104,12 +2110,6 @@
     <t>FBIDescription</t>
   </si>
   <si>
-    <t xml:space="preserve">A </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alaskan Native </t>
-  </si>
-  <si>
     <t>Chinese</t>
   </si>
   <si>
@@ -2134,9 +2134,6 @@
     <t>Other Pacific Islander</t>
   </si>
   <si>
-    <t>American Indian</t>
-  </si>
-  <si>
     <t>58</t>
   </si>
   <si>
@@ -2249,13 +2246,16 @@
   </si>
   <si>
     <t>Victim Was Ex-Relationship</t>
+  </si>
+  <si>
+    <t>American Indian/Alaskan Native</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -2313,15 +2313,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color auto="1"/>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2456,7 +2458,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2467,16 +2469,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="128">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -2606,13 +2610,16 @@
     <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="TableStyleLight1" xfId="1"/>
+    <cellStyle name="TableStyleLight1" xfId="1" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2904,14 +2911,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="41.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
@@ -3174,7 +3181,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B29">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B29">
     <sortCondition ref="A2:A29"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3188,14 +3195,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="49.6640625" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
@@ -3489,14 +3496,14 @@
       <c r="B15" s="1">
         <v>28</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>701</v>
+      <c r="C15" s="9" t="s">
+        <v>698</v>
       </c>
       <c r="D15" s="1">
         <v>28</v>
       </c>
-      <c r="E15" s="11" t="s">
-        <v>701</v>
+      <c r="E15" s="9" t="s">
+        <v>698</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>389</v>
@@ -3509,14 +3516,14 @@
       <c r="B16" s="1">
         <v>29</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>702</v>
+      <c r="C16" s="9" t="s">
+        <v>699</v>
       </c>
       <c r="D16" s="1">
         <v>29</v>
       </c>
-      <c r="E16" s="11" t="s">
-        <v>702</v>
+      <c r="E16" s="9" t="s">
+        <v>699</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>389</v>
@@ -3529,14 +3536,14 @@
       <c r="B17" s="1">
         <v>31</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>721</v>
+      <c r="C17" s="9" t="s">
+        <v>718</v>
       </c>
       <c r="D17" s="1">
         <v>31</v>
       </c>
-      <c r="E17" s="11" t="s">
-        <v>721</v>
+      <c r="E17" s="9" t="s">
+        <v>718</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>390</v>
@@ -3570,13 +3577,13 @@
         <v>33</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="D19" s="1">
         <v>33</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>390</v>
@@ -3809,14 +3816,14 @@
       <c r="B31" s="1">
         <v>81</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>703</v>
+      <c r="C31" s="9" t="s">
+        <v>700</v>
       </c>
       <c r="D31" s="1">
         <v>81</v>
       </c>
-      <c r="E31" s="11" t="s">
-        <v>703</v>
+      <c r="E31" s="9" t="s">
+        <v>700</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>389</v>
@@ -3829,14 +3836,14 @@
       <c r="B32" s="1">
         <v>82</v>
       </c>
-      <c r="C32" s="11" t="s">
-        <v>704</v>
+      <c r="C32" s="9" t="s">
+        <v>701</v>
       </c>
       <c r="D32" s="1">
         <v>82</v>
       </c>
-      <c r="E32" s="11" t="s">
-        <v>704</v>
+      <c r="E32" s="9" t="s">
+        <v>701</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>389</v>
@@ -3849,14 +3856,14 @@
       <c r="B33" s="1">
         <v>83</v>
       </c>
-      <c r="C33" s="11" t="s">
-        <v>705</v>
+      <c r="C33" s="9" t="s">
+        <v>702</v>
       </c>
       <c r="D33" s="1">
         <v>83</v>
       </c>
-      <c r="E33" s="11" t="s">
-        <v>705</v>
+      <c r="E33" s="9" t="s">
+        <v>702</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>389</v>
@@ -3869,14 +3876,14 @@
       <c r="B34" s="1">
         <v>84</v>
       </c>
-      <c r="C34" s="11" t="s">
-        <v>706</v>
+      <c r="C34" s="9" t="s">
+        <v>703</v>
       </c>
       <c r="D34" s="1">
         <v>84</v>
       </c>
-      <c r="E34" s="11" t="s">
-        <v>706</v>
+      <c r="E34" s="9" t="s">
+        <v>703</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>389</v>
@@ -3889,14 +3896,14 @@
       <c r="B35" s="1">
         <v>85</v>
       </c>
-      <c r="C35" s="11" t="s">
-        <v>707</v>
+      <c r="C35" s="9" t="s">
+        <v>704</v>
       </c>
       <c r="D35" s="1">
         <v>85</v>
       </c>
-      <c r="E35" s="11" t="s">
-        <v>707</v>
+      <c r="E35" s="9" t="s">
+        <v>704</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>389</v>
@@ -3974,14 +3981,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="3"/>
     <col min="3" max="3" width="29.33203125" customWidth="1"/>
@@ -4171,14 +4178,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="3"/>
     <col min="3" max="3" width="38.33203125" bestFit="1" customWidth="1"/>
@@ -5388,14 +5395,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="31.1640625" customWidth="1"/>
     <col min="4" max="4" width="32.33203125" customWidth="1"/>
@@ -5754,14 +5761,14 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="19.33203125" customWidth="1"/>
     <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
@@ -6017,14 +6024,14 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
@@ -6229,14 +6236,14 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="44.6640625" customWidth="1"/>
     <col min="5" max="5" width="43.33203125" bestFit="1" customWidth="1"/>
@@ -6267,13 +6274,13 @@
         <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>51</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
@@ -6403,13 +6410,13 @@
         <v>67</v>
       </c>
       <c r="C10" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>67</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1">
@@ -6492,14 +6499,14 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="74" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="74" bestFit="1" customWidth="1"/>
@@ -6687,14 +6694,14 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
@@ -6797,276 +6804,259 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="35.1640625" customWidth="1"/>
     <col min="5" max="5" width="34.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="13" t="s">
         <v>528</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="13" t="s">
         <v>681</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="13" t="s">
         <v>682</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="13" t="s">
         <v>683</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1">
-      <c r="A2">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="13" t="s">
         <v>373</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="13" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="13" t="s">
         <v>374</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="13" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1">
-      <c r="A4">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C4" t="s">
-        <v>694</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="C4" s="13" t="s">
+        <v>730</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="13" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="A5" s="13">
+        <v>5</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>684</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1">
+      <c r="A6" s="13">
+        <v>6</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6" s="13" t="s">
         <v>685</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A7" s="13">
+        <v>7</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>686</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E7" s="13" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>154</v>
-      </c>
-      <c r="C7" t="s">
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A8" s="13">
+        <v>8</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>687</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E8" s="13" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C8" s="8" t="s">
+    <row r="9" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A9" s="13">
+        <v>9</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>688</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E9" s="13" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="C9" s="8" t="s">
+    <row r="10" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A10" s="13">
+        <v>10</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>689</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C10" s="8" t="s">
+      <c r="D10" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1">
+      <c r="A11" s="13">
+        <v>11</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>690</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="C11" s="8" t="s">
+      <c r="D11" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A12" s="13">
+        <v>12</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>691</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D12" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E12" s="13" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>275</v>
-      </c>
-      <c r="C12" t="s">
-        <v>692</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>693</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1">
-      <c r="A14">
+    <row r="13" spans="1:5" ht="15" customHeight="1">
+      <c r="A13" s="13">
         <v>99999</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B13" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C13" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D13" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E13" s="13" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15">
+    <row r="14" spans="1:5">
+      <c r="A14" s="13">
         <v>99998</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B14" s="13" t="s">
         <v>501</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C14" s="13" t="s">
         <v>502</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D14" s="13" t="s">
         <v>501</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E14" s="13" t="s">
         <v>502</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C7">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C6">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -7080,14 +7070,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="26.5" customWidth="1"/>
     <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
@@ -7169,13 +7159,13 @@
         <v>246</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>246</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -7224,14 +7214,14 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
@@ -7334,14 +7324,14 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
@@ -7444,14 +7434,14 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="46.1640625" customWidth="1"/>
     <col min="5" max="5" width="34.83203125" bestFit="1" customWidth="1"/>
@@ -7567,13 +7557,13 @@
         <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
@@ -7809,14 +7799,14 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="63.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="63.5" bestFit="1" customWidth="1"/>
@@ -8004,14 +7994,14 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
@@ -8216,14 +8206,14 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="46" bestFit="1" customWidth="1"/>
@@ -8574,16 +8564,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1">
@@ -8591,16 +8581,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1">
@@ -8689,7 +8679,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C27">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C27">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -8703,14 +8693,14 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="19.1640625" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
@@ -8830,14 +8820,14 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
@@ -8940,14 +8930,14 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="25.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.83203125" bestFit="1" customWidth="1"/>
@@ -9152,14 +9142,14 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="25.33203125" customWidth="1"/>
     <col min="5" max="5" width="25.1640625" bestFit="1" customWidth="1"/>
@@ -9262,14 +9252,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="26.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.83203125" bestFit="1" customWidth="1"/>
@@ -9440,14 +9430,14 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="1"/>
     <col min="3" max="3" width="23.6640625" customWidth="1"/>
@@ -9670,14 +9660,14 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.1640625" bestFit="1" customWidth="1"/>
@@ -9742,13 +9732,13 @@
         <v>501</v>
       </c>
       <c r="C4" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>501</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -9780,14 +9770,14 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
@@ -10219,14 +10209,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="A58" sqref="A58:XFD58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="1"/>
     <col min="2" max="2" width="8.83203125" style="3"/>
@@ -11024,60 +11014,60 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="15" customHeight="1">
-      <c r="A28" s="12">
+      <c r="A28" s="10">
         <v>266</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="11" t="s">
         <v>651</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>716</v>
-      </c>
-      <c r="D28" s="13" t="s">
+      <c r="C28" s="10" t="s">
+        <v>713</v>
+      </c>
+      <c r="D28" s="11" t="s">
         <v>651</v>
       </c>
-      <c r="E28" s="12" t="s">
-        <v>716</v>
-      </c>
-      <c r="F28" s="12" t="s">
+      <c r="E28" s="10" t="s">
+        <v>713</v>
+      </c>
+      <c r="F28" s="10" t="s">
         <v>539</v>
       </c>
-      <c r="G28" s="12" t="s">
+      <c r="G28" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="H28" s="12" t="s">
+      <c r="H28" s="10" t="s">
         <v>582</v>
       </c>
-      <c r="I28" s="12" t="s">
+      <c r="I28" s="10" t="s">
         <v>558</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15" customHeight="1">
-      <c r="A29" s="12">
+      <c r="A29" s="10">
         <v>267</v>
       </c>
-      <c r="B29" s="13" t="s">
-        <v>714</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>715</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>714</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>715</v>
-      </c>
-      <c r="F29" s="12" t="s">
+      <c r="B29" s="11" t="s">
+        <v>711</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>712</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>711</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>712</v>
+      </c>
+      <c r="F29" s="10" t="s">
         <v>539</v>
       </c>
-      <c r="G29" s="12" t="s">
+      <c r="G29" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="H29" s="12" t="s">
+      <c r="H29" s="10" t="s">
         <v>582</v>
       </c>
-      <c r="I29" s="12" t="s">
+      <c r="I29" s="10" t="s">
         <v>558</v>
       </c>
     </row>
@@ -11437,13 +11427,13 @@
         <v>616</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>616</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>539</v>
@@ -11466,13 +11456,13 @@
         <v>618</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>618</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>539</v>
@@ -11495,13 +11485,13 @@
         <v>619</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>619</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>539</v>
@@ -11524,13 +11514,13 @@
         <v>620</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>620</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>539</v>
@@ -11582,13 +11572,13 @@
         <v>622</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>622</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>539</v>
@@ -11611,13 +11601,13 @@
         <v>624</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>624</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>539</v>
@@ -11898,16 +11888,16 @@
         <v>909</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>628</v>
@@ -12184,7 +12174,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C63">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C63">
     <sortCondition ref="A2:A63"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -12198,14 +12188,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35" bestFit="1" customWidth="1"/>
@@ -12253,13 +12243,13 @@
         <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1">
@@ -12342,14 +12332,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="3"/>
     <col min="3" max="3" width="43.5" customWidth="1"/>
@@ -12670,13 +12660,13 @@
         <v>85</v>
       </c>
       <c r="C19" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>85</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1">
@@ -13143,16 +13133,16 @@
         <v>58</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -13201,14 +13191,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
@@ -13311,14 +13301,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="31.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.83203125" bestFit="1" customWidth="1"/>
@@ -13349,13 +13339,13 @@
         <v>37</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
@@ -13434,13 +13424,13 @@
         <v>140</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>140</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
@@ -13468,13 +13458,13 @@
         <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1">
@@ -13535,13 +13525,13 @@
       <c r="B13" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="8" t="s">
         <v>149</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="8" t="s">
         <v>149</v>
       </c>
     </row>
@@ -13552,14 +13542,14 @@
       <c r="B14" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>700</v>
+      <c r="C14" s="8" t="s">
+        <v>697</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>700</v>
+      <c r="E14" s="8" t="s">
+        <v>697</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1">
@@ -13642,14 +13632,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="3"/>
     <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
@@ -13800,13 +13790,13 @@
         <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="D9" s="2">
         <v>35</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1">

</xml_diff>